<commit_message>
InputPrep.py corr. & input data corr.
</commit_message>
<xml_diff>
--- a/migforecasting/less100/input prep/smallinput.xlsx
+++ b/migforecasting/less100/input prep/smallinput.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -104,6 +104,12 @@
   <si>
     <t>Гуково</t>
   </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
 </sst>
 </file>
 
@@ -142,12 +148,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +190,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +497,10 @@
     <col min="12" max="12" width="14.5703125" customWidth="1"/>
     <col min="13" max="13" width="18.5703125" customWidth="1"/>
     <col min="14" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,10 +541,16 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -549,17 +573,16 @@
         <v>31.7</v>
       </c>
       <c r="H2" s="2">
-        <f xml:space="preserve"> 2188679 / 1000</f>
-        <v>2188.6790000000001</v>
+        <v>42.934637189320675</v>
       </c>
       <c r="I2" s="2">
         <f xml:space="preserve"> 34115239 / 1000</f>
         <v>34115.239000000001</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="2">
@@ -571,10 +594,16 @@
         <v>90.087999999999994</v>
       </c>
       <c r="N2" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O2" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P2" s="2">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -597,8 +626,7 @@
         <v>31.7</v>
       </c>
       <c r="H3" s="2">
-        <f xml:space="preserve"> 1171317 / 1000</f>
-        <v>1171.317</v>
+        <v>24.79712507409603</v>
       </c>
       <c r="I3" s="2">
         <f xml:space="preserve"> 35242373 / 1000</f>
@@ -608,7 +636,7 @@
         <f xml:space="preserve"> 3936 / 1000</f>
         <v>3.9359999999999999</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L3" s="2">
@@ -620,10 +648,16 @@
         <v>136.577</v>
       </c>
       <c r="N3" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O3" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P3" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -646,7 +680,7 @@
         <v>31.7</v>
       </c>
       <c r="H4" s="2">
-        <v>1156.5740000000001</v>
+        <v>24.071220446220448</v>
       </c>
       <c r="I4" s="2">
         <v>35244.355000000003</v>
@@ -655,7 +689,7 @@
         <f xml:space="preserve"> 5651769 / 1000</f>
         <v>5651.7690000000002</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="2">
@@ -665,10 +699,16 @@
         <v>886.95799999999997</v>
       </c>
       <c r="N4" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O4" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P4" s="2">
         <v>-39</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -691,7 +731,7 @@
         <v>31.7</v>
       </c>
       <c r="H5" s="2">
-        <v>1532.6489999999999</v>
+        <v>31.519773778920307</v>
       </c>
       <c r="I5" s="2">
         <v>28569.743999999999</v>
@@ -699,7 +739,7 @@
       <c r="J5" s="3">
         <v>1633.874</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L5" s="2">
@@ -709,10 +749,16 @@
         <v>799.875</v>
       </c>
       <c r="N5" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O5" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -735,7 +781,7 @@
         <v>31.7</v>
       </c>
       <c r="H6" s="2">
-        <v>1979.982</v>
+        <v>40.197783011206752</v>
       </c>
       <c r="I6" s="2">
         <v>27686.793000000001</v>
@@ -743,7 +789,7 @@
       <c r="J6" s="2">
         <v>4598.3109999999997</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="2">
@@ -753,10 +799,16 @@
         <v>358.774</v>
       </c>
       <c r="N6" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O6" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P6" s="2">
         <v>-99</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -779,7 +831,7 @@
         <v>31.7</v>
       </c>
       <c r="H7" s="2">
-        <v>1362.4960000000001</v>
+        <v>27.239568963793761</v>
       </c>
       <c r="I7" s="2">
         <v>25606.316999999999</v>
@@ -787,20 +839,26 @@
       <c r="J7" s="2">
         <v>2782.0369999999998</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="2">
         <v>1784.922</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="N7" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O7" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P7" s="2">
         <v>-186</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -823,7 +881,7 @@
         <v>31.3</v>
       </c>
       <c r="H8" s="2">
-        <v>1631.1479999999999</v>
+        <v>32.356343727683885</v>
       </c>
       <c r="I8" s="2">
         <v>22342.066999999999</v>
@@ -831,20 +889,26 @@
       <c r="J8" s="2">
         <v>193.648</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L8" s="2">
         <v>1761.789</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="N8" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O8" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P8" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -867,7 +931,7 @@
         <v>30.7</v>
       </c>
       <c r="H9" s="2">
-        <v>894.31299999999999</v>
+        <v>17.619847899755694</v>
       </c>
       <c r="I9" s="2">
         <v>22261.996999999999</v>
@@ -885,10 +949,16 @@
         <v>14.432</v>
       </c>
       <c r="N9" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O9" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P9" s="2">
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -911,7 +981,7 @@
         <v>36.43</v>
       </c>
       <c r="H10" s="2">
-        <v>1381.8050000000001</v>
+        <v>26.93682014893368</v>
       </c>
       <c r="I10" s="2">
         <v>19849.96</v>
@@ -929,10 +999,16 @@
         <v>17.542000000000002</v>
       </c>
       <c r="N10" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O10" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P10" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -955,7 +1031,7 @@
         <v>36.43</v>
       </c>
       <c r="H11" s="2">
-        <v>814.22699999999998</v>
+        <v>15.675997766696828</v>
       </c>
       <c r="I11" s="2">
         <v>17254.972000000002</v>
@@ -973,10 +1049,16 @@
         <v>16.149000000000001</v>
       </c>
       <c r="N11" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O11" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P11" s="2">
         <v>-257</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1081,7 @@
         <v>36.43</v>
       </c>
       <c r="H12" s="2">
-        <v>691.16099999999994</v>
+        <v>13.205215896064194</v>
       </c>
       <c r="I12" s="2">
         <v>17653.433000000001</v>
@@ -1017,10 +1099,16 @@
         <v>24.484999999999999</v>
       </c>
       <c r="N12" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O12" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P12" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1131,7 @@
         <v>36.43</v>
       </c>
       <c r="H13" s="2">
-        <v>955.6</v>
+        <v>18.045169574741294</v>
       </c>
       <c r="I13" s="2">
         <v>16316.396500000001</v>
@@ -1061,10 +1149,16 @@
         <v>32.409999999999997</v>
       </c>
       <c r="N13" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O13" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P13" s="2">
         <v>-76</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1087,7 +1181,7 @@
         <v>36.43</v>
       </c>
       <c r="H14" s="2">
-        <v>577.28300000000002</v>
+        <v>10.823109227942554</v>
       </c>
       <c r="I14" s="2">
         <v>15980.2601</v>
@@ -1105,10 +1199,16 @@
         <v>29.247</v>
       </c>
       <c r="N14" s="2">
+        <v>59.8</v>
+      </c>
+      <c r="O14" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="P14" s="2">
         <v>-150</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1131,7 +1231,7 @@
         <v>25.9</v>
       </c>
       <c r="H15" s="3">
-        <v>8534.4</v>
+        <v>35.856111722642822</v>
       </c>
       <c r="I15" s="3">
         <v>98966.3</v>
@@ -1151,10 +1251,16 @@
         <v>353.488</v>
       </c>
       <c r="N15" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P15" s="2">
         <v>-3761</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1283,7 @@
         <v>25.9</v>
       </c>
       <c r="H16" s="3">
-        <v>19293.900000000001</v>
+        <v>79.343257803182965</v>
       </c>
       <c r="I16" s="3">
         <v>81900</v>
@@ -1197,10 +1303,16 @@
         <v>171.5384</v>
       </c>
       <c r="N16" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P16" s="2">
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -1223,7 +1335,7 @@
         <v>25.9</v>
       </c>
       <c r="H17" s="3">
-        <v>6649.3</v>
+        <v>27.222445119504787</v>
       </c>
       <c r="I17" s="3">
         <v>63344.5</v>
@@ -1243,10 +1355,16 @@
         <v>132.601</v>
       </c>
       <c r="N17" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P17" s="2">
         <v>-63</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -1269,7 +1387,7 @@
         <v>25.9</v>
       </c>
       <c r="H18" s="3">
-        <v>7320.8</v>
+        <v>29.807089403353341</v>
       </c>
       <c r="I18" s="3">
         <v>60117.7</v>
@@ -1289,10 +1407,16 @@
         <v>128.20910000000001</v>
       </c>
       <c r="N18" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O18" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P18" s="2">
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -1315,7 +1439,7 @@
         <v>25.9</v>
       </c>
       <c r="H19" s="3">
-        <v>7689.2</v>
+        <v>31.256910569105692</v>
       </c>
       <c r="I19" s="3">
         <v>57475.199999999997</v>
@@ -1333,10 +1457,16 @@
         <v>722</v>
       </c>
       <c r="N19" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O19" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P19" s="2">
         <v>942</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1359,8 +1489,7 @@
         <v>25.9</v>
       </c>
       <c r="H20" s="3">
-        <f xml:space="preserve"> 4558593 / 1000</f>
-        <v>4558.5929999999998</v>
+        <v>18.515812347684811</v>
       </c>
       <c r="I20" s="3">
         <f xml:space="preserve"> 41975492 / 1000</f>
@@ -1382,10 +1511,16 @@
         <v>119.837</v>
       </c>
       <c r="N20" s="2">
+        <v>59.2</v>
+      </c>
+      <c r="O20" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="P20" s="2">
         <v>3215</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1408,15 +1543,15 @@
         <v>25.9</v>
       </c>
       <c r="H21" s="3">
-        <v>3022.6</v>
+        <v>32.969741922816816</v>
       </c>
       <c r="I21" s="3">
         <v>22280.27</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L21" s="3">
@@ -1428,10 +1563,16 @@
         <v>333.72520000000003</v>
       </c>
       <c r="N21" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="O21" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="P21" s="2">
         <v>-1280</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
@@ -1454,15 +1595,15 @@
         <v>25.9</v>
       </c>
       <c r="H22" s="3">
-        <v>12843.2</v>
+        <v>137.03506113825998</v>
       </c>
       <c r="I22" s="3">
         <v>33385.4</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L22" s="3">
@@ -1474,10 +1615,16 @@
         <v>170.054</v>
       </c>
       <c r="N22" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="O22" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="P22" s="2">
         <v>-28</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -1500,15 +1647,15 @@
         <v>25.9</v>
       </c>
       <c r="H23" s="3">
-        <v>2983.3</v>
+        <v>31.586024351508737</v>
       </c>
       <c r="I23" s="3">
         <v>26147.7</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L23" s="3">
@@ -1520,10 +1667,16 @@
         <v>130.23500000000001</v>
       </c>
       <c r="N23" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="O23" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="P23" s="2">
         <v>-114</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>19</v>
       </c>
@@ -1546,15 +1699,15 @@
         <v>25.9</v>
       </c>
       <c r="H24" s="3">
-        <v>4169.8</v>
+        <v>43.810544453550193</v>
       </c>
       <c r="I24" s="3">
         <v>25080.5</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L24" s="3">
@@ -1566,10 +1719,16 @@
         <v>123.943</v>
       </c>
       <c r="N24" s="2">
+        <v>59.3</v>
+      </c>
+      <c r="O24" s="2">
+        <v>30.07</v>
+      </c>
+      <c r="P24" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>20</v>
       </c>
@@ -1592,8 +1751,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H25" s="3">
-        <f>32741549/1000</f>
-        <v>32741.548999999999</v>
+        <v>168.16150239082089</v>
       </c>
       <c r="I25" s="3">
         <f xml:space="preserve"> 188.5 * 1000</f>
@@ -1613,10 +1771,16 @@
         <v>859</v>
       </c>
       <c r="N25" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O25" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P25" s="2">
         <v>516</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>20</v>
       </c>
@@ -1639,8 +1803,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H26" s="3">
-        <f>22754436/1000</f>
-        <v>22754.436000000002</v>
+        <v>118.16987177822672</v>
       </c>
       <c r="I26" s="3">
         <f xml:space="preserve"> 172 * 1000</f>
@@ -1661,10 +1824,16 @@
         <v>775.67230000000006</v>
       </c>
       <c r="N26" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O26" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P26" s="2">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -1687,8 +1856,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H27" s="3">
-        <f>19495388/1000</f>
-        <v>19495.387999999999</v>
+        <v>100.58138443044571</v>
       </c>
       <c r="I27" s="3">
         <f xml:space="preserve"> 152.7 * 1000</f>
@@ -1709,10 +1877,16 @@
         <v>710.65710000000001</v>
       </c>
       <c r="N27" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O27" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P27" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -1735,7 +1909,7 @@
         <v>29.3</v>
       </c>
       <c r="H28" s="3">
-        <v>37458.699999999997</v>
+        <v>191.27879366603176</v>
       </c>
       <c r="I28" s="3">
         <f xml:space="preserve"> 110.9 * 1000</f>
@@ -1757,10 +1931,16 @@
         <v>368.78840000000002</v>
       </c>
       <c r="N28" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O28" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P28" s="2">
         <v>-907</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
@@ -1783,8 +1963,7 @@
         <v>28.6</v>
       </c>
       <c r="H29" s="3">
-        <f>21049559/1000</f>
-        <v>21049.559000000001</v>
+        <v>106.18809054174717</v>
       </c>
       <c r="I29" s="3">
         <f>101*1000</f>
@@ -1806,10 +1985,16 @@
         <v>482.38299999999998</v>
       </c>
       <c r="N29" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O29" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P29" s="2">
         <v>-212</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
@@ -1832,8 +2017,7 @@
         <v>27.5</v>
       </c>
       <c r="H30" s="3">
-        <f>26707512/1000</f>
-        <v>26707.511999999999</v>
+        <v>133.79779671460992</v>
       </c>
       <c r="I30" s="3">
         <f>105.7*1000</f>
@@ -1855,10 +2039,16 @@
         <v>114.82769999999999</v>
       </c>
       <c r="N30" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O30" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P30" s="2">
         <v>-440</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>20</v>
       </c>
@@ -1881,8 +2071,7 @@
         <v>26.9</v>
       </c>
       <c r="H31" s="3">
-        <f>7232770/1000</f>
-        <v>7232.77</v>
+        <v>35.942444541623601</v>
       </c>
       <c r="I31" s="3">
         <f>65.7 *1000</f>
@@ -1903,10 +2092,16 @@
         <v>76.884299999999996</v>
       </c>
       <c r="N31" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O31" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P31" s="2">
         <v>-550</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
@@ -1929,16 +2124,15 @@
         <v>27.3</v>
       </c>
       <c r="H32" s="3">
-        <f>12749153/1000</f>
-        <v>12749.153</v>
+        <v>172.03245219878829</v>
       </c>
       <c r="I32" s="3">
         <v>49354.7</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="8">
         <v>0</v>
       </c>
       <c r="L32" s="3">
@@ -1950,10 +2144,16 @@
         <v>319.74619999999999</v>
       </c>
       <c r="N32" s="2">
+        <v>60.4</v>
+      </c>
+      <c r="O32" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="P32" s="2">
         <v>-543</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
@@ -1976,28 +2176,34 @@
         <v>15</v>
       </c>
       <c r="H33" s="3">
-        <v>945.42700000000002</v>
+        <v>27.847628865979381</v>
       </c>
       <c r="I33" s="3">
         <v>9164.8922000000002</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L33" s="3">
         <v>747.80160000000001</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M33" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N33" s="2">
+        <v>59.07</v>
+      </c>
+      <c r="O33" s="2">
+        <v>28.05</v>
+      </c>
+      <c r="P33" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>22</v>
       </c>
@@ -2020,28 +2226,34 @@
         <v>15</v>
       </c>
       <c r="H34" s="2">
-        <v>782.58500000000004</v>
+        <v>22.869228521332555</v>
       </c>
       <c r="I34" s="2">
         <v>9026.0113999999994</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="J34" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L34" s="2">
         <v>352.14210000000003</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="M34" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N34" s="2">
+        <v>59.07</v>
+      </c>
+      <c r="O34" s="2">
+        <v>28.05</v>
+      </c>
+      <c r="P34" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>24</v>
       </c>
@@ -2064,7 +2276,7 @@
         <v>26.5</v>
       </c>
       <c r="H35" s="2">
-        <v>807.98599999999999</v>
+        <v>39.033140096618361</v>
       </c>
       <c r="I35" s="6">
         <f xml:space="preserve"> 258584 / 1000</f>
@@ -2083,10 +2295,16 @@
         <v>52.4</v>
       </c>
       <c r="N35" s="2">
+        <v>48.01</v>
+      </c>
+      <c r="O35" s="2">
+        <v>40.07</v>
+      </c>
+      <c r="P35" s="2">
         <v>-261</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>24</v>
       </c>
@@ -2109,10 +2327,11 @@
         <v>25.9</v>
       </c>
       <c r="H36" s="2">
-        <v>749.79399999999998</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>15</v>
+        <v>35.535260663507103</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" ref="I36:I39" si="0" xml:space="preserve"> 258584 / 1000</f>
+        <v>258.584</v>
       </c>
       <c r="J36" s="2">
         <v>96.450999999999993</v>
@@ -2127,10 +2346,16 @@
         <v>50</v>
       </c>
       <c r="N36" s="2">
+        <v>48.01</v>
+      </c>
+      <c r="O36" s="2">
+        <v>40.07</v>
+      </c>
+      <c r="P36" s="2">
         <v>-329</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>24</v>
       </c>
@@ -2153,10 +2378,11 @@
         <v>25.3</v>
       </c>
       <c r="H37" s="2">
-        <v>854.34799999999996</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>15</v>
+        <v>39.553148148148146</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="0"/>
+        <v>258.584</v>
       </c>
       <c r="J37" s="2">
         <v>25.128</v>
@@ -2171,10 +2397,16 @@
         <v>52</v>
       </c>
       <c r="N37" s="2">
+        <v>48.01</v>
+      </c>
+      <c r="O37" s="2">
+        <v>40.07</v>
+      </c>
+      <c r="P37" s="2">
         <v>-407</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>24</v>
       </c>
@@ -2197,10 +2429,11 @@
         <v>24.7</v>
       </c>
       <c r="H38" s="2">
-        <v>633.245</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>15</v>
+        <v>28.653619909502261</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="0"/>
+        <v>258.584</v>
       </c>
       <c r="J38" s="2">
         <v>99.796000000000006</v>
@@ -2215,10 +2448,16 @@
         <v>56.5</v>
       </c>
       <c r="N38" s="2">
+        <v>48.01</v>
+      </c>
+      <c r="O38" s="2">
+        <v>40.07</v>
+      </c>
+      <c r="P38" s="2">
         <v>-394</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>24</v>
       </c>
@@ -2241,10 +2480,11 @@
         <v>24</v>
       </c>
       <c r="H39" s="2">
-        <v>1442.961</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>15</v>
+        <v>63.566563876651983</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="0"/>
+        <v>258.584</v>
       </c>
       <c r="J39" s="2">
         <v>29.158000000000001</v>
@@ -2259,10 +2499,16 @@
         <v>51.9</v>
       </c>
       <c r="N39" s="2">
+        <v>48.01</v>
+      </c>
+      <c r="O39" s="2">
+        <v>40.07</v>
+      </c>
+      <c r="P39" s="2">
         <v>-412</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>25</v>
       </c>
@@ -2285,7 +2531,7 @@
         <v>24.9</v>
       </c>
       <c r="H40" s="2">
-        <v>404.32</v>
+        <v>8.4585774058577403</v>
       </c>
       <c r="I40" s="6">
         <f xml:space="preserve"> 2342648 / 1000</f>
@@ -2304,10 +2550,16 @@
         <v>135</v>
       </c>
       <c r="N40" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="O40" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P40" s="2">
         <v>-361</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>25</v>
       </c>
@@ -2330,10 +2582,11 @@
         <v>20</v>
       </c>
       <c r="H41" s="2">
-        <v>453.06599999999997</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>15</v>
+        <v>9.3608677685950408</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" ref="I41:I44" si="1" xml:space="preserve"> 2342648 / 1000</f>
+        <v>2342.6480000000001</v>
       </c>
       <c r="J41" s="2">
         <v>138.08099999999999</v>
@@ -2348,10 +2601,16 @@
         <v>126.6</v>
       </c>
       <c r="N41" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="O41" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P41" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>25</v>
       </c>
@@ -2374,10 +2633,11 @@
         <v>21.5</v>
       </c>
       <c r="H42" s="2">
-        <v>554.66600000000005</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>15</v>
+        <v>11.389445585215606</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="1"/>
+        <v>2342.6480000000001</v>
       </c>
       <c r="J42" s="2">
         <v>153.685</v>
@@ -2392,10 +2652,16 @@
         <v>129.1</v>
       </c>
       <c r="N42" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="O42" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P42" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>25</v>
       </c>
@@ -2418,10 +2684,11 @@
         <v>21.5</v>
       </c>
       <c r="H43" s="2">
-        <v>945.928</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>15</v>
+        <v>19.304653061224489</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="1"/>
+        <v>2342.6480000000001</v>
       </c>
       <c r="J43" s="2">
         <v>137.809</v>
@@ -2436,10 +2703,16 @@
         <v>135.9</v>
       </c>
       <c r="N43" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="O43" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P43" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>25</v>
       </c>
@@ -2462,10 +2735,11 @@
         <v>21.3</v>
       </c>
       <c r="H44" s="2">
-        <v>836.05100000000004</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>15</v>
+        <v>16.99290650406504</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="1"/>
+        <v>2342.6480000000001</v>
       </c>
       <c r="J44" s="2">
         <v>225.78100000000001</v>
@@ -2480,10 +2754,16 @@
         <v>124.3</v>
       </c>
       <c r="N44" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="O44" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P44" s="2">
         <v>-72</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>26</v>
       </c>
@@ -2506,7 +2786,7 @@
         <v>22.2</v>
       </c>
       <c r="H45" s="2">
-        <v>3089.9859999999999</v>
+        <v>34.718943820224716</v>
       </c>
       <c r="I45" s="6">
         <f xml:space="preserve"> 22314234 / 1000</f>
@@ -2525,10 +2805,16 @@
         <v>715.1</v>
       </c>
       <c r="N45" s="2">
+        <v>48.19</v>
+      </c>
+      <c r="O45" s="2">
+        <v>40.1</v>
+      </c>
+      <c r="P45" s="2">
         <v>-91</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>26</v>
       </c>
@@ -2551,10 +2837,11 @@
         <v>21.8</v>
       </c>
       <c r="H46" s="2">
-        <v>2497.1320000000001</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>15</v>
+        <v>27.869776785714286</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" ref="I46:I49" si="2" xml:space="preserve"> 22314234 / 1000</f>
+        <v>22314.234</v>
       </c>
       <c r="J46" s="2">
         <v>1519.3689999999999</v>
@@ -2569,10 +2856,16 @@
         <v>673.3</v>
       </c>
       <c r="N46" s="2">
+        <v>48.19</v>
+      </c>
+      <c r="O46" s="2">
+        <v>40.1</v>
+      </c>
+      <c r="P46" s="2">
         <v>-208</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
@@ -2595,10 +2888,11 @@
         <v>21.6</v>
       </c>
       <c r="H47" s="2">
-        <v>1752.0909999999999</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>15</v>
+        <v>19.403001107419712</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="2"/>
+        <v>22314.234</v>
       </c>
       <c r="J47" s="2">
         <v>1571.5360000000001</v>
@@ -2613,10 +2907,16 @@
         <v>687.9</v>
       </c>
       <c r="N47" s="2">
+        <v>48.19</v>
+      </c>
+      <c r="O47" s="2">
+        <v>40.1</v>
+      </c>
+      <c r="P47" s="2">
         <v>-469</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>26</v>
       </c>
@@ -2639,10 +2939,11 @@
         <v>21.3</v>
       </c>
       <c r="H48" s="2">
-        <v>1704.595</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>15</v>
+        <v>18.690734649122806</v>
+      </c>
+      <c r="I48" s="7">
+        <f t="shared" si="2"/>
+        <v>22314.234</v>
       </c>
       <c r="J48" s="2">
         <v>1291.039</v>
@@ -2657,10 +2958,16 @@
         <v>670.7</v>
       </c>
       <c r="N48" s="2">
+        <v>48.19</v>
+      </c>
+      <c r="O48" s="2">
+        <v>40.1</v>
+      </c>
+      <c r="P48" s="2">
         <v>-388</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>26</v>
       </c>
@@ -2683,10 +2990,11 @@
         <v>21</v>
       </c>
       <c r="H49" s="2">
-        <v>1383.492</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>15</v>
+        <v>15.03795652173913</v>
+      </c>
+      <c r="I49" s="7">
+        <f t="shared" si="2"/>
+        <v>22314.234</v>
       </c>
       <c r="J49" s="2">
         <v>950.87800000000004</v>
@@ -2701,10 +3009,16 @@
         <v>617.1</v>
       </c>
       <c r="N49" s="2">
+        <v>48.19</v>
+      </c>
+      <c r="O49" s="2">
+        <v>40.1</v>
+      </c>
+      <c r="P49" s="2">
         <v>-589</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>27</v>
       </c>
@@ -2727,7 +3041,7 @@
         <v>22.4</v>
       </c>
       <c r="H50" s="2">
-        <v>643.65099999999995</v>
+        <v>9.9175808936825867</v>
       </c>
       <c r="I50" s="6">
         <f xml:space="preserve"> 1824354 / 1000</f>
@@ -2746,10 +3060,16 @@
         <v>215.7</v>
       </c>
       <c r="N50" s="2">
+        <v>48.03</v>
+      </c>
+      <c r="O50" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P50" s="2">
         <v>-887</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>27</v>
       </c>
@@ -2772,10 +3092,11 @@
         <v>22.2</v>
       </c>
       <c r="H51" s="2">
-        <v>532.17899999999997</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>15</v>
+        <v>8.0268325791855197</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" ref="I51:I54" si="3" xml:space="preserve"> 1824354 / 1000</f>
+        <v>1824.354</v>
       </c>
       <c r="J51" s="2">
         <v>437.738</v>
@@ -2790,10 +3111,16 @@
         <v>206.4</v>
       </c>
       <c r="N51" s="2">
+        <v>48.03</v>
+      </c>
+      <c r="O51" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P51" s="2">
         <v>1081</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>27</v>
       </c>
@@ -2816,10 +3143,11 @@
         <v>22.3</v>
       </c>
       <c r="H52" s="2">
-        <v>1074.3510000000001</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>15</v>
+        <v>16.352374429223744</v>
+      </c>
+      <c r="I52" s="7">
+        <f t="shared" si="3"/>
+        <v>1824.354</v>
       </c>
       <c r="J52" s="2">
         <v>529.05600000000004</v>
@@ -2834,10 +3162,16 @@
         <v>217.4</v>
       </c>
       <c r="N52" s="2">
+        <v>48.03</v>
+      </c>
+      <c r="O52" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P52" s="2">
         <v>731</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>27</v>
       </c>
@@ -2860,10 +3194,11 @@
         <v>22.2</v>
       </c>
       <c r="H53" s="2">
-        <v>734.88400000000001</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>15</v>
+        <v>11.236758409785931</v>
+      </c>
+      <c r="I53" s="7">
+        <f t="shared" si="3"/>
+        <v>1824.354</v>
       </c>
       <c r="J53" s="2">
         <v>611.07500000000005</v>
@@ -2878,10 +3213,16 @@
         <v>215.5</v>
       </c>
       <c r="N53" s="2">
+        <v>48.03</v>
+      </c>
+      <c r="O53" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P53" s="2">
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>27</v>
       </c>
@@ -2904,10 +3245,11 @@
         <v>22.2</v>
       </c>
       <c r="H54" s="2">
-        <v>721.66300000000001</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>15</v>
+        <v>11.051500765696785</v>
+      </c>
+      <c r="I54" s="7">
+        <f t="shared" si="3"/>
+        <v>1824.354</v>
       </c>
       <c r="J54" s="2">
         <v>626.43600000000004</v>
@@ -2922,10 +3264,16 @@
         <v>197.6</v>
       </c>
       <c r="N54" s="2">
+        <v>48.03</v>
+      </c>
+      <c r="O54" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="P54" s="2">
         <v>-171</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>23</v>
       </c>
@@ -2948,13 +3296,13 @@
         <v>15</v>
       </c>
       <c r="H55" s="2">
-        <v>3672</v>
+        <v>45.785536159600994</v>
       </c>
       <c r="I55" s="2">
         <f xml:space="preserve"> 28823135 / 1000</f>
         <v>28823.134999999998</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="J55" s="8" t="s">
         <v>15</v>
       </c>
       <c r="K55" s="3">
@@ -2967,10 +3315,16 @@
         <v>413.2</v>
       </c>
       <c r="N55" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O55" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P55" s="2">
         <v>-51</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>23</v>
       </c>
@@ -2993,7 +3347,7 @@
         <v>24.3</v>
       </c>
       <c r="H56" s="2">
-        <v>6245.3890000000001</v>
+        <v>77.390198265179677</v>
       </c>
       <c r="I56" s="6">
         <f xml:space="preserve"> 32671949 / 1000</f>
@@ -3012,10 +3366,16 @@
         <v>399.8</v>
       </c>
       <c r="N56" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O56" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P56" s="2">
         <v>-460</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>23</v>
       </c>
@@ -3038,10 +3398,11 @@
         <v>23.3</v>
       </c>
       <c r="H57" s="2">
-        <v>5762.2879999999996</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>15</v>
+        <v>70.876851168511678</v>
+      </c>
+      <c r="I57" s="7">
+        <f t="shared" ref="I57:I60" si="4" xml:space="preserve"> 32671949 / 1000</f>
+        <v>32671.949000000001</v>
       </c>
       <c r="J57" s="2">
         <v>1185.2070000000001</v>
@@ -3056,10 +3417,16 @@
         <v>376.7</v>
       </c>
       <c r="N57" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O57" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P57" s="2">
         <v>-342</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>23</v>
       </c>
@@ -3082,10 +3449,11 @@
         <v>22.4</v>
       </c>
       <c r="H58" s="2">
-        <v>4329.107</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>15</v>
+        <v>52.858449328449325</v>
+      </c>
+      <c r="I58" s="7">
+        <f t="shared" si="4"/>
+        <v>32671.949000000001</v>
       </c>
       <c r="J58" s="2">
         <v>1524.723</v>
@@ -3100,10 +3468,16 @@
         <v>379</v>
       </c>
       <c r="N58" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O58" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P58" s="2">
         <v>-98</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>23</v>
       </c>
@@ -3126,10 +3500,11 @@
         <v>21.6</v>
       </c>
       <c r="H59" s="2">
-        <v>4719.0659999999998</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>15</v>
+        <v>57.549585365853659</v>
+      </c>
+      <c r="I59" s="7">
+        <f t="shared" si="4"/>
+        <v>32671.949000000001</v>
       </c>
       <c r="J59" s="2">
         <v>900.72900000000004</v>
@@ -3144,10 +3519,16 @@
         <v>366.4</v>
       </c>
       <c r="N59" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O59" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P59" s="2">
         <v>-331</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>23</v>
       </c>
@@ -3170,10 +3551,11 @@
         <v>21</v>
       </c>
       <c r="H60" s="2">
-        <v>4947.8760000000002</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>15</v>
+        <v>59.974254545454549</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" si="4"/>
+        <v>32671.949000000001</v>
       </c>
       <c r="J60" s="2">
         <v>401.06799999999998</v>
@@ -3188,10 +3570,16 @@
         <v>335.2</v>
       </c>
       <c r="N60" s="2">
+        <v>47.06</v>
+      </c>
+      <c r="O60" s="2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="P60" s="2">
         <v>-213</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="2"/>

</xml_diff>

<commit_message>
Input small cities (next year)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/input prep/smallinput.xlsx
+++ b/migforecasting/less100/input prep/smallinput.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,7 +2172,7 @@
       <c r="F33" s="2">
         <v>28993.5</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H33" s="3">
@@ -2222,7 +2222,7 @@
       <c r="F34" s="2">
         <v>26864.3</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H34" s="2">
@@ -3292,8 +3292,8 @@
       <c r="F55" s="2">
         <v>29249.1</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>15</v>
+      <c r="G55" s="8">
+        <v>24.3</v>
       </c>
       <c r="H55" s="2">
         <v>45.785536159600994</v>

</xml_diff>